<commit_message>
rebrand from devkit to TAL Platform and add new modules
</commit_message>
<xml_diff>
--- a/seeds/schemas/accounts.xlsx
+++ b/seeds/schemas/accounts.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="columns_mapper" sheetId="1" state="visible" r:id="rId3"/>
@@ -540,7 +540,7 @@
     <t xml:space="preserve">0 1118614244</t>
   </si>
   <si>
-    <t xml:space="preserve">ahmed@devkit.com</t>
+    <t xml:space="preserve">ahmed@devkit.comtalplatformai</t>
   </si>
   <si>
     <t xml:space="preserve">super admin</t>
@@ -552,7 +552,7 @@
     <t xml:space="preserve">kareem</t>
   </si>
   <si>
-    <t xml:space="preserve">kareem@devkit.com</t>
+    <t xml:space="preserve">kareem@devkit.comtalplatformai</t>
   </si>
   <si>
     <t xml:space="preserve">images/avatar2.webp</t>
@@ -565,7 +565,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -606,6 +606,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -663,12 +671,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -678,10 +690,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -701,6 +709,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -978,58 +990,58 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1065,16 +1077,16 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1088,7 +1100,7 @@
       <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1127,7 +1139,7 @@
       <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1135,13 +1147,13 @@
       <c r="A2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7"/>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1207,231 +1219,239 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1456,8 +1476,8 @@
   </sheetPr>
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1474,611 +1494,611 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="2" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="2" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="2" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" s="2" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I15" s="2" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="2" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="2" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I18" s="2" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I20" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I21" s="2" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2101,10 +2121,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2118,39 +2138,39 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>170</v>
       </c>
       <c r="E2" s="8" t="n">
@@ -2159,21 +2179,21 @@
       <c r="F2" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="4" t="n">
         <v>1202290100</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>174</v>
       </c>
       <c r="E3" s="8" t="n">
@@ -2182,17 +2202,19 @@
       <c r="F3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F5" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D8" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="ahmed@devkit.com"/>
-    <hyperlink ref="D3" r:id="rId2" display="kareem@devkit.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>